<commit_message>
cuarta forma normal implentada
</commit_message>
<xml_diff>
--- a/Normalizacion_Proyecto.xlsx
+++ b/Normalizacion_Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\OneDrive\Documentos\Bases de Datos 1\Proyecto\Database-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131B6253-9B42-4EB1-8E4E-369C94D5199B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A16D6F-6EF9-4BFA-A475-C35BD3E1A322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C36F66E8-2FBE-49EE-BFDE-FBC2E57B799F}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{C36F66E8-2FBE-49EE-BFDE-FBC2E57B799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="89">
   <si>
     <t>Actividad_cod</t>
   </si>
@@ -267,13 +267,46 @@
   </si>
   <si>
     <t>Tercera Forma Normal</t>
+  </si>
+  <si>
+    <t>Cuarta Forma Normal</t>
+  </si>
+  <si>
+    <t>sala_id</t>
+  </si>
+  <si>
+    <t>clase_de_alumno_id</t>
+  </si>
+  <si>
+    <t>persona_id</t>
+  </si>
+  <si>
+    <t>Actividades</t>
+  </si>
+  <si>
+    <t>salas</t>
+  </si>
+  <si>
+    <t>clases</t>
+  </si>
+  <si>
+    <t>personas</t>
+  </si>
+  <si>
+    <t>usuarios</t>
+  </si>
+  <si>
+    <t>alumnos</t>
+  </si>
+  <si>
+    <t>clase_de_alumno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +343,14 @@
       <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -521,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -567,9 +608,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,7 +635,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -882,19 +931,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC5D224-BE37-45B0-873A-72853BECF1FF}">
-  <dimension ref="A1:Z38"/>
+  <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="7" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" customWidth="1"/>
@@ -915,12 +965,12 @@
     <col min="26" max="26" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -967,7 +1017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1061,7 +1111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -1108,7 +1158,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -1155,13 +1205,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A8" s="32" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="32"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>0</v>
       </c>
@@ -1177,59 +1227,62 @@
       <c r="F10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="M10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="26" t="s">
+      <c r="N10" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="O10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="P10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="Q10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="22" t="s">
+      <c r="S10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="22" t="s">
+      <c r="T10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T10" s="28" t="s">
+      <c r="U10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="23" t="s">
+      <c r="V10" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="W10" s="17" t="s">
+      <c r="X10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="X10" s="22" t="s">
+      <c r="Y10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="Y10" s="26" t="s">
+      <c r="Z10" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1245,59 +1298,62 @@
       <c r="F11" s="3">
         <v>15</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="7">
         <v>44190.416666666664</v>
       </c>
-      <c r="J11" s="3">
-        <v>1</v>
-      </c>
       <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
         <v>117530123</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="M11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="N11" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="27" t="s">
+      <c r="O11" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="24">
+      <c r="P11" s="24">
         <v>35818</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="12">
-        <v>1</v>
-      </c>
       <c r="S11" s="12">
+        <v>1</v>
+      </c>
+      <c r="T11" s="12">
         <v>117530175</v>
       </c>
-      <c r="T11" s="12" t="s">
+      <c r="U11" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="U11" s="3" t="s">
+      <c r="V11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="V11" s="3" t="s">
+      <c r="W11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="W11" s="19">
+      <c r="X11" s="19">
         <v>36402</v>
       </c>
-      <c r="X11" s="12" t="s">
+      <c r="Y11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Y11" s="27" t="s">
+      <c r="Z11" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -1313,59 +1369,62 @@
       <c r="F12" s="3">
         <v>7</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="8">
+      <c r="I12" s="8">
         <v>44189.375</v>
       </c>
-      <c r="J12" s="3">
-        <v>2</v>
-      </c>
       <c r="K12" s="3">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
         <v>589329112</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="N12" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="O12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="O12" s="24">
+      <c r="P12" s="24">
         <v>32999</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="R12" s="12">
-        <v>2</v>
-      </c>
       <c r="S12" s="12">
+        <v>2</v>
+      </c>
+      <c r="T12" s="12">
         <v>503960247</v>
       </c>
-      <c r="T12" s="12" t="s">
+      <c r="U12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="U12" s="3" t="s">
+      <c r="V12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="V12" s="3" t="s">
+      <c r="W12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="W12" s="19">
+      <c r="X12" s="19">
         <v>34303</v>
       </c>
-      <c r="X12" s="12" t="s">
+      <c r="Y12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y12" s="27" t="s">
+      <c r="Z12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -1381,59 +1440,62 @@
       <c r="F13" s="6">
         <v>14</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="9">
+      <c r="I13" s="9">
         <v>44188.333333333336</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <v>3</v>
       </c>
-      <c r="K13" s="6">
+      <c r="L13" s="6">
         <v>230293202</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="M13" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M13" s="27" t="s">
+      <c r="N13" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="N13" s="27" t="s">
+      <c r="O13" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="O13" s="25">
+      <c r="P13" s="25">
         <v>34278</v>
       </c>
-      <c r="P13" s="6" t="s">
+      <c r="Q13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R13" s="13">
+      <c r="S13" s="13">
         <v>3</v>
       </c>
-      <c r="S13" s="13">
+      <c r="T13" s="13">
         <v>502220222</v>
       </c>
-      <c r="T13" s="12" t="s">
+      <c r="U13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="U13" s="3" t="s">
+      <c r="V13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="V13" s="3" t="s">
+      <c r="W13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="W13" s="20">
+      <c r="X13" s="20">
         <v>35945</v>
       </c>
-      <c r="X13" s="12" t="s">
+      <c r="Y13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="Y13" s="27" t="s">
+      <c r="Z13" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>4</v>
       </c>
@@ -1449,59 +1511,62 @@
       <c r="F14" s="3">
         <v>13</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="3">
+        <v>4</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="7">
+      <c r="I14" s="7">
         <v>44188.416666666664</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>4</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>523123212</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="M14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="M14" s="27" t="s">
+      <c r="N14" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="N14" s="27" t="s">
+      <c r="O14" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="O14" s="24">
+      <c r="P14" s="24">
         <v>36870</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R14" s="12">
+      <c r="S14" s="12">
         <v>4</v>
       </c>
-      <c r="S14" s="12">
+      <c r="T14" s="12">
         <v>501110111</v>
       </c>
-      <c r="T14" s="12" t="s">
+      <c r="U14" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="V14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="W14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="W14" s="19">
+      <c r="X14" s="19">
         <v>36505</v>
       </c>
-      <c r="X14" s="12" t="s">
+      <c r="Y14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Y14" s="27" t="s">
+      <c r="Z14" s="27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A16" s="32" t="s">
         <v>74</v>
       </c>
@@ -2226,73 +2291,618 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="31"/>
       <c r="D33" s="31"/>
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E34" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="G34" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="H34" s="21" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E35" s="3">
         <v>1</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7">
         <v>44190.416666666664</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E36" s="3">
         <v>2</v>
       </c>
       <c r="F36" s="3">
         <v>2</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="3">
+        <v>2</v>
+      </c>
+      <c r="H36" s="8">
         <v>44189.375</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E37" s="6">
         <v>3</v>
       </c>
       <c r="F37" s="6">
         <v>3</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="6">
+        <v>3</v>
+      </c>
+      <c r="H37" s="9">
         <v>44188.333333333336</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E38" s="3">
         <v>4</v>
       </c>
       <c r="F38" s="3">
         <v>4</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="3">
+        <v>4</v>
+      </c>
+      <c r="H38" s="7">
         <v>44188.416666666664</v>
       </c>
     </row>
+    <row r="42" spans="1:19" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A42" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="32"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M45" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="3">
+        <v>20</v>
+      </c>
+      <c r="F46" s="3">
+        <v>15</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="7">
+        <v>44190.416666666664</v>
+      </c>
+      <c r="M46" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="N46" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="O46" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P46" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q46" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="R46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="S46" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>2</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="3">
+        <v>7</v>
+      </c>
+      <c r="F47" s="3">
+        <v>7</v>
+      </c>
+      <c r="G47" s="3">
+        <v>2</v>
+      </c>
+      <c r="H47" s="3">
+        <v>1</v>
+      </c>
+      <c r="I47" s="8">
+        <v>44189.375</v>
+      </c>
+      <c r="M47" s="3">
+        <v>1</v>
+      </c>
+      <c r="N47" s="3">
+        <v>117530123</v>
+      </c>
+      <c r="O47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P47" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q47" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="R47" s="33">
+        <v>35818</v>
+      </c>
+      <c r="S47" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>3</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="6">
+        <v>15</v>
+      </c>
+      <c r="F48" s="6">
+        <v>14</v>
+      </c>
+      <c r="G48" s="6">
+        <v>3</v>
+      </c>
+      <c r="H48" s="6">
+        <v>2</v>
+      </c>
+      <c r="I48" s="9">
+        <v>44188.333333333336</v>
+      </c>
+      <c r="M48" s="3">
+        <v>2</v>
+      </c>
+      <c r="N48" s="3">
+        <v>589329112</v>
+      </c>
+      <c r="O48" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="P48" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q48" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="R48" s="33">
+        <v>32999</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>4</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="3">
+        <v>15</v>
+      </c>
+      <c r="F49" s="3">
+        <v>13</v>
+      </c>
+      <c r="G49" s="3">
+        <v>4</v>
+      </c>
+      <c r="H49" s="3">
+        <v>3</v>
+      </c>
+      <c r="I49" s="7">
+        <v>44188.416666666664</v>
+      </c>
+      <c r="M49" s="6">
+        <v>3</v>
+      </c>
+      <c r="N49" s="6">
+        <v>230293202</v>
+      </c>
+      <c r="O49" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="P49" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q49" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="R49" s="34">
+        <v>34278</v>
+      </c>
+      <c r="S49" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M50" s="3">
+        <v>4</v>
+      </c>
+      <c r="N50" s="3">
+        <v>523123212</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="P50" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q50" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="R50" s="33">
+        <v>36870</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M51" s="12">
+        <v>5</v>
+      </c>
+      <c r="N51" s="12">
+        <v>117530175</v>
+      </c>
+      <c r="O51" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R51" s="19">
+        <v>36402</v>
+      </c>
+      <c r="S51" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E52" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="H52" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="M52" s="12">
+        <v>6</v>
+      </c>
+      <c r="N52" s="12">
+        <v>503960247</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R52" s="19">
+        <v>34303</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E53" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="I53" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="J53" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M53" s="13">
+        <v>7</v>
+      </c>
+      <c r="N53" s="13">
+        <v>502220222</v>
+      </c>
+      <c r="O53" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R53" s="20">
+        <v>35945</v>
+      </c>
+      <c r="S53" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <v>1</v>
+      </c>
+      <c r="K54" s="7">
+        <v>44190.416666666664</v>
+      </c>
+      <c r="M54" s="12">
+        <v>8</v>
+      </c>
+      <c r="N54" s="12">
+        <v>501110111</v>
+      </c>
+      <c r="O54" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R54" s="19">
+        <v>36505</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E55" s="6">
+        <v>2</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H55" s="3">
+        <v>2</v>
+      </c>
+      <c r="I55" s="3">
+        <v>2</v>
+      </c>
+      <c r="J55" s="3">
+        <v>2</v>
+      </c>
+      <c r="K55" s="8">
+        <v>44189.375</v>
+      </c>
+      <c r="M55" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q55" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E56" s="3">
+        <v>3</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H56" s="6">
+        <v>3</v>
+      </c>
+      <c r="I56" s="6">
+        <v>3</v>
+      </c>
+      <c r="J56" s="6">
+        <v>2</v>
+      </c>
+      <c r="K56" s="9">
+        <v>44188.333333333336</v>
+      </c>
+      <c r="M56" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="N56" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="O56" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q56" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="R56" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H57" s="3">
+        <v>4</v>
+      </c>
+      <c r="I57" s="3">
+        <v>4</v>
+      </c>
+      <c r="J57" s="3">
+        <v>4</v>
+      </c>
+      <c r="K57" s="7">
+        <v>44188.416666666664</v>
+      </c>
+      <c r="M57" s="12">
+        <v>5</v>
+      </c>
+      <c r="N57" s="12">
+        <v>1</v>
+      </c>
+      <c r="O57" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q57" s="3">
+        <v>1</v>
+      </c>
+      <c r="R57" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M58" s="12">
+        <v>6</v>
+      </c>
+      <c r="N58" s="12">
+        <v>2</v>
+      </c>
+      <c r="O58" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>2</v>
+      </c>
+      <c r="R58" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M59" s="13">
+        <v>7</v>
+      </c>
+      <c r="N59" s="13">
+        <v>3</v>
+      </c>
+      <c r="O59" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q59" s="6">
+        <v>3</v>
+      </c>
+      <c r="R59" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M60" s="12">
+        <v>8</v>
+      </c>
+      <c r="N60" s="12">
+        <v>4</v>
+      </c>
+      <c r="O60" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q60" s="3">
+        <v>4</v>
+      </c>
+      <c r="R60" s="12">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
columna precio agregada a la normalizacion
</commit_message>
<xml_diff>
--- a/Normalizacion_Proyecto.xlsx
+++ b/Normalizacion_Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\OneDrive\Documentos\Bases de Datos 1\Proyecto\Database-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A16D6F-6EF9-4BFA-A475-C35BD3E1A322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639673C7-E839-4A91-8072-11FB75805F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{C36F66E8-2FBE-49EE-BFDE-FBC2E57B799F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="90">
   <si>
     <t>Actividad_cod</t>
   </si>
@@ -300,13 +300,16 @@
   </si>
   <si>
     <t>clase_de_alumno</t>
+  </si>
+  <si>
+    <t>precio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +351,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -562,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -605,9 +617,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,6 +625,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
@@ -931,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC5D224-BE37-45B0-873A-72853BECF1FF}">
-  <dimension ref="A1:Z60"/>
+  <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,12 +980,12 @@
     <col min="26" max="26" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -984,40 +999,43 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1030,41 +1048,44 @@
       <c r="D3" s="3">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>44190.416666666664</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>117530123</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="5">
         <v>35818</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>117530175</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="19">
+      <c r="N3" s="19">
         <v>36402</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="O3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="P3" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1077,41 +1098,44 @@
       <c r="D4" s="3">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="8">
         <v>44189.375</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>589329112</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>32999</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="12">
+      <c r="L4" s="12">
         <v>503960247</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="19">
+      <c r="N4" s="19">
         <v>34303</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="O4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -1124,41 +1148,44 @@
       <c r="D5" s="6">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="6">
+        <v>1500</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>44188.333333333336</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <v>230293202</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="10">
         <v>34278</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="13">
+      <c r="L5" s="13">
         <v>502220222</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="20">
+      <c r="N5" s="20">
         <v>35945</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="O5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="P5" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -1171,47 +1198,50 @@
       <c r="D6" s="3">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>44188.416666666664</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>523123212</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>36870</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="12">
+      <c r="L6" s="12">
         <v>501110111</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="19">
+      <c r="N6" s="19">
         <v>36505</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="O6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="P6" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:27" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A8" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="32"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="36"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>0</v>
       </c>
@@ -1230,59 +1260,62 @@
       <c r="G10" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="M10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="N10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="O10" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="O10" s="26" t="s">
+      <c r="P10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="Q10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="R10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="22" t="s">
+      <c r="T10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T10" s="22" t="s">
+      <c r="U10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="28" t="s">
+      <c r="V10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="V10" s="23" t="s">
+      <c r="W10" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="X10" s="17" t="s">
+      <c r="Y10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="Y10" s="22" t="s">
+      <c r="Z10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="Z10" s="26" t="s">
+      <c r="AA10" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1301,59 +1334,62 @@
       <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="3">
+        <v>1500</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>44190.416666666664</v>
       </c>
-      <c r="K11" s="3">
-        <v>1</v>
-      </c>
       <c r="L11" s="3">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
         <v>117530123</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="N11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="27" t="s">
+      <c r="O11" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="27" t="s">
+      <c r="P11" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P11" s="24">
+      <c r="Q11" s="24">
         <v>35818</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="12">
-        <v>1</v>
-      </c>
       <c r="T11" s="12">
+        <v>1</v>
+      </c>
+      <c r="U11" s="12">
         <v>117530175</v>
       </c>
-      <c r="U11" s="12" t="s">
+      <c r="V11" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="V11" s="3" t="s">
+      <c r="W11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W11" s="3" t="s">
+      <c r="X11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X11" s="19">
+      <c r="Y11" s="19">
         <v>36402</v>
       </c>
-      <c r="Y11" s="12" t="s">
+      <c r="Z11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Z11" s="27" t="s">
+      <c r="AA11" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -1372,59 +1408,62 @@
       <c r="G12" s="3">
         <v>2</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="3">
+        <v>5000</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="8">
+      <c r="J12" s="8">
         <v>44189.375</v>
       </c>
-      <c r="K12" s="3">
-        <v>2</v>
-      </c>
       <c r="L12" s="3">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
         <v>589329112</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="N12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="O12" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="27" t="s">
+      <c r="P12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="P12" s="24">
+      <c r="Q12" s="24">
         <v>32999</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S12" s="12">
-        <v>2</v>
-      </c>
       <c r="T12" s="12">
+        <v>2</v>
+      </c>
+      <c r="U12" s="12">
         <v>503960247</v>
       </c>
-      <c r="U12" s="12" t="s">
+      <c r="V12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="V12" s="3" t="s">
+      <c r="W12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="X12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="X12" s="19">
+      <c r="Y12" s="19">
         <v>34303</v>
       </c>
-      <c r="Y12" s="12" t="s">
+      <c r="Z12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Z12" s="27" t="s">
+      <c r="AA12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -1443,59 +1482,62 @@
       <c r="G13" s="6">
         <v>3</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="9">
+      <c r="J13" s="9">
         <v>44188.333333333336</v>
       </c>
-      <c r="K13" s="6">
+      <c r="L13" s="6">
         <v>3</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <v>230293202</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="N13" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="N13" s="27" t="s">
+      <c r="O13" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="O13" s="27" t="s">
+      <c r="P13" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="P13" s="25">
+      <c r="Q13" s="25">
         <v>34278</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="R13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="13">
+      <c r="T13" s="13">
         <v>3</v>
       </c>
-      <c r="T13" s="13">
+      <c r="U13" s="13">
         <v>502220222</v>
       </c>
-      <c r="U13" s="12" t="s">
+      <c r="V13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="V13" s="3" t="s">
+      <c r="W13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="W13" s="3" t="s">
+      <c r="X13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="X13" s="20">
+      <c r="Y13" s="20">
         <v>35945</v>
       </c>
-      <c r="Y13" s="12" t="s">
+      <c r="Z13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="Z13" s="27" t="s">
+      <c r="AA13" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>4</v>
       </c>
@@ -1514,65 +1556,68 @@
       <c r="G14" s="3">
         <v>4</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="7">
+      <c r="J14" s="7">
         <v>44188.416666666664</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>4</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>523123212</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="N14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="N14" s="27" t="s">
+      <c r="O14" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="O14" s="27" t="s">
+      <c r="P14" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P14" s="24">
+      <c r="Q14" s="24">
         <v>36870</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="R14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S14" s="12">
+      <c r="T14" s="12">
         <v>4</v>
       </c>
-      <c r="T14" s="12">
+      <c r="U14" s="12">
         <v>501110111</v>
       </c>
-      <c r="U14" s="12" t="s">
+      <c r="V14" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="W14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="X14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="X14" s="19">
+      <c r="Y14" s="19">
         <v>36505</v>
       </c>
-      <c r="Y14" s="12" t="s">
+      <c r="Z14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Z14" s="27" t="s">
+      <c r="AA14" s="27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A16" s="32" t="s">
+    <row r="16" spans="1:27" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A16" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="32"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>0</v>
       </c>
@@ -1591,59 +1636,62 @@
       <c r="G18" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="J18" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="L18" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="21" t="s">
+      <c r="M18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="22" t="s">
+      <c r="N18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N18" s="26" t="s">
+      <c r="O18" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="O18" s="26" t="s">
+      <c r="P18" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="P18" s="16" t="s">
+      <c r="Q18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q18" s="21" t="s">
+      <c r="R18" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="S18" s="22" t="s">
+      <c r="T18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T18" s="22" t="s">
+      <c r="U18" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="28" t="s">
+      <c r="V18" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="V18" s="23" t="s">
+      <c r="W18" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="W18" s="23" t="s">
+      <c r="X18" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="X18" s="17" t="s">
+      <c r="Y18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="Y18" s="21" t="s">
+      <c r="Z18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Z18" s="16" t="s">
+      <c r="AA18" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -1662,59 +1710,62 @@
       <c r="G19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="3">
+        <v>1500</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="7">
+      <c r="J19" s="7">
         <v>44190.416666666664</v>
       </c>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
       <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3">
         <v>117530123</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="N19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="27" t="s">
+      <c r="O19" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="O19" s="27" t="s">
+      <c r="P19" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P19" s="24">
+      <c r="Q19" s="24">
         <v>35818</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="R19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S19" s="12">
-        <v>1</v>
-      </c>
       <c r="T19" s="12">
+        <v>1</v>
+      </c>
+      <c r="U19" s="12">
         <v>117530175</v>
       </c>
-      <c r="U19" s="12" t="s">
+      <c r="V19" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="V19" s="3" t="s">
+      <c r="W19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W19" s="3" t="s">
+      <c r="X19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X19" s="19">
+      <c r="Y19" s="19">
         <v>36402</v>
       </c>
-      <c r="Y19" s="3" t="s">
+      <c r="Z19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z19" s="14" t="s">
+      <c r="AA19" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -1733,59 +1784,62 @@
       <c r="G20" s="3">
         <v>2</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="3">
+        <v>5000</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="8">
+      <c r="J20" s="8">
         <v>44189.375</v>
       </c>
-      <c r="K20" s="3">
-        <v>2</v>
-      </c>
       <c r="L20" s="3">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
         <v>589329112</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="N20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="27" t="s">
+      <c r="O20" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="27" t="s">
+      <c r="P20" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="P20" s="24">
+      <c r="Q20" s="24">
         <v>32999</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="R20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S20" s="12">
-        <v>2</v>
-      </c>
       <c r="T20" s="12">
+        <v>2</v>
+      </c>
+      <c r="U20" s="12">
         <v>503960247</v>
       </c>
-      <c r="U20" s="12" t="s">
+      <c r="V20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="V20" s="3" t="s">
+      <c r="W20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="W20" s="3" t="s">
+      <c r="X20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="X20" s="19">
+      <c r="Y20" s="19">
         <v>34303</v>
       </c>
-      <c r="Y20" s="3" t="s">
+      <c r="Z20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z20" s="14" t="s">
+      <c r="AA20" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>3</v>
       </c>
@@ -1804,59 +1858,62 @@
       <c r="G21" s="6">
         <v>3</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="9">
+      <c r="J21" s="9">
         <v>44188.333333333336</v>
       </c>
-      <c r="K21" s="6">
+      <c r="L21" s="6">
         <v>3</v>
       </c>
-      <c r="L21" s="6">
+      <c r="M21" s="6">
         <v>230293202</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="N21" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="N21" s="27" t="s">
+      <c r="O21" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="27" t="s">
+      <c r="P21" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="P21" s="25">
+      <c r="Q21" s="25">
         <v>34278</v>
       </c>
-      <c r="Q21" s="6" t="s">
+      <c r="R21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S21" s="13">
+      <c r="T21" s="13">
         <v>3</v>
       </c>
-      <c r="T21" s="13">
+      <c r="U21" s="13">
         <v>502220222</v>
       </c>
-      <c r="U21" s="12" t="s">
+      <c r="V21" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="V21" s="3" t="s">
+      <c r="W21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="X21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="X21" s="20">
+      <c r="Y21" s="20">
         <v>35945</v>
       </c>
-      <c r="Y21" s="3" t="s">
+      <c r="Z21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Z21" s="15" t="s">
+      <c r="AA21" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>4</v>
       </c>
@@ -1875,68 +1932,71 @@
       <c r="G22" s="3">
         <v>4</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="7">
+      <c r="J22" s="7">
         <v>44188.416666666664</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>4</v>
       </c>
-      <c r="L22" s="3">
+      <c r="M22" s="3">
         <v>523123212</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="N22" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="N22" s="27" t="s">
+      <c r="O22" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="O22" s="27" t="s">
+      <c r="P22" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P22" s="24">
+      <c r="Q22" s="24">
         <v>36870</v>
       </c>
-      <c r="Q22" s="3" t="s">
+      <c r="R22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S22" s="12">
+      <c r="T22" s="12">
         <v>4</v>
       </c>
-      <c r="T22" s="12">
+      <c r="U22" s="12">
         <v>501110111</v>
       </c>
-      <c r="U22" s="12" t="s">
+      <c r="V22" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="V22" s="3" t="s">
+      <c r="W22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="W22" s="3" t="s">
+      <c r="X22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="X22" s="19">
+      <c r="Y22" s="19">
         <v>36505</v>
       </c>
-      <c r="Y22" s="3" t="s">
+      <c r="Z22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z22" s="14" t="s">
+      <c r="AA22" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="F24" s="29"/>
     </row>
-    <row r="25" spans="1:26" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A25" s="32" t="s">
+    <row r="25" spans="1:27" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A25" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="32"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>0</v>
       </c>
@@ -1955,59 +2015,62 @@
       <c r="G27" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="J27" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="K27" s="21" t="s">
+      <c r="L27" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L27" s="21" t="s">
+      <c r="M27" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="22" t="s">
+      <c r="N27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="26" t="s">
+      <c r="O27" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="O27" s="26" t="s">
+      <c r="P27" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="P27" s="16" t="s">
+      <c r="Q27" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="21" t="s">
+      <c r="R27" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="S27" s="22" t="s">
+      <c r="T27" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T27" s="22" t="s">
+      <c r="U27" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="U27" s="28" t="s">
+      <c r="V27" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="V27" s="23" t="s">
+      <c r="W27" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="W27" s="23" t="s">
+      <c r="X27" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="X27" s="17" t="s">
+      <c r="Y27" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="Y27" s="21" t="s">
+      <c r="Z27" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Z27" s="16" t="s">
+      <c r="AA27" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1</v>
       </c>
@@ -2026,59 +2089,62 @@
       <c r="G28" s="3">
         <v>1</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="3">
+        <v>1500</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="7">
+      <c r="J28" s="7">
         <v>44190.416666666664</v>
       </c>
-      <c r="K28" s="3">
-        <v>1</v>
-      </c>
       <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="3">
         <v>117530123</v>
       </c>
-      <c r="M28" s="12" t="s">
+      <c r="N28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="N28" s="27" t="s">
+      <c r="O28" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="O28" s="27" t="s">
+      <c r="P28" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P28" s="24">
+      <c r="Q28" s="24">
         <v>35818</v>
       </c>
-      <c r="Q28" s="3" t="s">
+      <c r="R28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S28" s="12">
-        <v>1</v>
-      </c>
       <c r="T28" s="12">
+        <v>1</v>
+      </c>
+      <c r="U28" s="12">
         <v>117530175</v>
       </c>
-      <c r="U28" s="12" t="s">
+      <c r="V28" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="V28" s="3" t="s">
+      <c r="W28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W28" s="3" t="s">
+      <c r="X28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X28" s="19">
+      <c r="Y28" s="19">
         <v>36402</v>
       </c>
-      <c r="Y28" s="3" t="s">
+      <c r="Z28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z28" s="14" t="s">
+      <c r="AA28" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -2097,59 +2163,62 @@
       <c r="G29" s="3">
         <v>2</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="3">
+        <v>5000</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="8">
+      <c r="J29" s="8">
         <v>44189.375</v>
       </c>
-      <c r="K29" s="3">
-        <v>2</v>
-      </c>
       <c r="L29" s="3">
+        <v>2</v>
+      </c>
+      <c r="M29" s="3">
         <v>589329112</v>
       </c>
-      <c r="M29" s="12" t="s">
+      <c r="N29" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="N29" s="27" t="s">
+      <c r="O29" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="O29" s="27" t="s">
+      <c r="P29" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="P29" s="24">
+      <c r="Q29" s="24">
         <v>32999</v>
       </c>
-      <c r="Q29" s="3" t="s">
+      <c r="R29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S29" s="12">
-        <v>2</v>
-      </c>
       <c r="T29" s="12">
+        <v>2</v>
+      </c>
+      <c r="U29" s="12">
         <v>503960247</v>
       </c>
-      <c r="U29" s="12" t="s">
+      <c r="V29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="V29" s="3" t="s">
+      <c r="W29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="W29" s="3" t="s">
+      <c r="X29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="X29" s="19">
+      <c r="Y29" s="19">
         <v>34303</v>
       </c>
-      <c r="Y29" s="3" t="s">
+      <c r="Z29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z29" s="14" t="s">
+      <c r="AA29" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>3</v>
       </c>
@@ -2168,59 +2237,62 @@
       <c r="G30" s="6">
         <v>3</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="6">
+        <v>1500</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="9">
+      <c r="J30" s="9">
         <v>44188.333333333336</v>
       </c>
-      <c r="K30" s="6">
+      <c r="L30" s="6">
         <v>3</v>
       </c>
-      <c r="L30" s="6">
+      <c r="M30" s="6">
         <v>230293202</v>
       </c>
-      <c r="M30" s="13" t="s">
+      <c r="N30" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="N30" s="27" t="s">
+      <c r="O30" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="O30" s="27" t="s">
+      <c r="P30" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="25">
+      <c r="Q30" s="25">
         <v>34278</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S30" s="13">
+      <c r="T30" s="13">
         <v>3</v>
       </c>
-      <c r="T30" s="13">
+      <c r="U30" s="13">
         <v>502220222</v>
       </c>
-      <c r="U30" s="12" t="s">
+      <c r="V30" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="V30" s="3" t="s">
+      <c r="W30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="W30" s="3" t="s">
+      <c r="X30" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="X30" s="20">
+      <c r="Y30" s="20">
         <v>35945</v>
       </c>
-      <c r="Y30" s="3" t="s">
+      <c r="Z30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Z30" s="15" t="s">
+      <c r="AA30" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>4</v>
       </c>
@@ -2239,55 +2311,58 @@
       <c r="G31" s="3">
         <v>4</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I31" s="7">
+      <c r="J31" s="7">
         <v>44188.416666666664</v>
       </c>
-      <c r="K31" s="3">
+      <c r="L31" s="3">
         <v>4</v>
       </c>
-      <c r="L31" s="3">
+      <c r="M31" s="3">
         <v>523123212</v>
       </c>
-      <c r="M31" s="12" t="s">
+      <c r="N31" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="N31" s="27" t="s">
+      <c r="O31" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="O31" s="27" t="s">
+      <c r="P31" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P31" s="24">
+      <c r="Q31" s="24">
         <v>36870</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="R31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S31" s="12">
+      <c r="T31" s="12">
         <v>4</v>
       </c>
-      <c r="T31" s="12">
+      <c r="U31" s="12">
         <v>501110111</v>
       </c>
-      <c r="U31" s="12" t="s">
+      <c r="V31" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="V31" s="3" t="s">
+      <c r="W31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="W31" s="3" t="s">
+      <c r="X31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="X31" s="19">
+      <c r="Y31" s="19">
         <v>36505</v>
       </c>
-      <c r="Y31" s="3" t="s">
+      <c r="Z31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z31" s="14" t="s">
+      <c r="AA31" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2369,16 +2444,16 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="36"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="34" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2401,13 +2476,16 @@
       <c r="G45" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="I45" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I45" s="21" t="s">
+      <c r="J45" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="M45" s="35" t="s">
+      <c r="M45" s="34" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2430,10 +2508,13 @@
       <c r="G46" s="3">
         <v>1</v>
       </c>
-      <c r="H46" s="3">
-        <v>1</v>
-      </c>
-      <c r="I46" s="7">
+      <c r="H46" s="38">
+        <v>1500</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+      <c r="J46" s="7">
         <v>44190.416666666664</v>
       </c>
       <c r="M46" s="21" t="s">
@@ -2477,10 +2558,13 @@
       <c r="G47" s="3">
         <v>2</v>
       </c>
-      <c r="H47" s="3">
-        <v>1</v>
-      </c>
-      <c r="I47" s="8">
+      <c r="H47" s="38">
+        <v>5000</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1</v>
+      </c>
+      <c r="J47" s="8">
         <v>44189.375</v>
       </c>
       <c r="M47" s="3">
@@ -2498,7 +2582,7 @@
       <c r="Q47" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="R47" s="33">
+      <c r="R47" s="32">
         <v>35818</v>
       </c>
       <c r="S47" s="3" t="s">
@@ -2524,10 +2608,13 @@
       <c r="G48" s="6">
         <v>3</v>
       </c>
-      <c r="H48" s="6">
-        <v>2</v>
-      </c>
-      <c r="I48" s="9">
+      <c r="H48" s="39">
+        <v>1500</v>
+      </c>
+      <c r="I48" s="6">
+        <v>2</v>
+      </c>
+      <c r="J48" s="9">
         <v>44188.333333333336</v>
       </c>
       <c r="M48" s="3">
@@ -2545,7 +2632,7 @@
       <c r="Q48" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="R48" s="33">
+      <c r="R48" s="32">
         <v>32999</v>
       </c>
       <c r="S48" s="3" t="s">
@@ -2571,10 +2658,13 @@
       <c r="G49" s="3">
         <v>4</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="38">
+        <v>2000</v>
+      </c>
+      <c r="I49" s="3">
         <v>3</v>
       </c>
-      <c r="I49" s="7">
+      <c r="J49" s="7">
         <v>44188.416666666664</v>
       </c>
       <c r="M49" s="6">
@@ -2592,7 +2682,7 @@
       <c r="Q49" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="R49" s="34">
+      <c r="R49" s="33">
         <v>34278</v>
       </c>
       <c r="S49" s="6" t="s">
@@ -2615,7 +2705,7 @@
       <c r="Q50" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="R50" s="33">
+      <c r="R50" s="32">
         <v>36870</v>
       </c>
       <c r="S50" s="3" t="s">
@@ -2646,10 +2736,10 @@
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E52" s="35" t="s">
+      <c r="E52" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="H52" s="35" t="s">
+      <c r="H52" s="34" t="s">
         <v>88</v>
       </c>
       <c r="M52" s="12">
@@ -2775,10 +2865,10 @@
       <c r="K55" s="8">
         <v>44189.375</v>
       </c>
-      <c r="M55" s="35" t="s">
+      <c r="M55" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="Q55" s="36" t="s">
+      <c r="Q55" s="35" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>